<commit_message>
finished all rating curves, updated environmental data, worked on modeling data
</commit_message>
<xml_diff>
--- a/Kriddie/october data.xlsx
+++ b/Kriddie/october data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kriddie\OneDrive - University of North Carolina at Chapel Hill\Documents\Ecuador2022\Kriddie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Kriddie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B4EEB74-FCEF-4CEE-8A8A-EF41DE0BE581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE074D19-52F1-0341-85AC-7C9EFBD26240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28875" yWindow="465" windowWidth="23865" windowHeight="14595" xr2:uid="{10B11F7C-B9A3-4F02-922F-71D45B566055}"/>
+    <workbookView xWindow="1940" yWindow="3320" windowWidth="35840" windowHeight="20300" xr2:uid="{10B11F7C-B9A3-4F02-922F-71D45B566055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>Wetland</t>
   </si>
@@ -78,54 +78,6 @@
   </si>
   <si>
     <t>AirTemp_C</t>
-  </si>
-  <si>
-    <t>AirPress_hpa</t>
-  </si>
-  <si>
-    <t>CO2_ppm</t>
-  </si>
-  <si>
-    <t>AirPress_atm</t>
-  </si>
-  <si>
-    <t>VaporPressure_atm</t>
-  </si>
-  <si>
-    <t>TotalAir_atm</t>
-  </si>
-  <si>
-    <t>Total_air_MolperL</t>
-  </si>
-  <si>
-    <t>CO2_air_MolesPerLiter</t>
-  </si>
-  <si>
-    <t>CO2_air_gCO2asCPerLiter</t>
-  </si>
-  <si>
-    <t>Watertemp_K</t>
-  </si>
-  <si>
-    <t>KH_mol.L.atm</t>
-  </si>
-  <si>
-    <t>CO2_water_gCO2asCPerLiter</t>
-  </si>
-  <si>
-    <t>deltaCO2_gCO2asCperM3</t>
-  </si>
-  <si>
-    <t>Flux_gCO2asCperM2perDay</t>
-  </si>
-  <si>
-    <t>k_m.d</t>
-  </si>
-  <si>
-    <t>Sc</t>
-  </si>
-  <si>
-    <t>K600</t>
   </si>
   <si>
     <t>Vial_no_ch4</t>
@@ -156,18 +108,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -188,17 +134,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,22 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B271F42-3A39-442A-9858-77021A957BC9}">
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,13 +495,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -577,128 +524,85 @@
       <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44740</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5">
-        <v>0.43402777777777773</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-    </row>
-    <row r="3" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44849</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.16211719999999999</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7.9491670000000001</v>
+      </c>
+      <c r="F2">
+        <v>274.16950000000003</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="I2">
+        <v>162</v>
+      </c>
+      <c r="L2" s="4">
+        <f>AVERAGE(-0.05,-0.02,-0.05)</f>
+        <v>-0.04</v>
+      </c>
+      <c r="M2" s="4">
+        <f>STDEV(-0.05,-0.02,-0.05)</f>
+        <v>1.732050807568877E-2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="O2">
+        <v>62.5518</v>
+      </c>
+      <c r="P2">
+        <v>6.9039999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>44849</v>
       </c>
       <c r="F3">
-        <v>274.16950000000003</v>
+        <v>270.22030000000001</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2">
-        <v>0.48055555555555557</v>
+        <v>0.48680555555555555</v>
       </c>
       <c r="I3">
-        <v>162</v>
-      </c>
-      <c r="L3" s="7">
-        <v>-8.1818180000000004E-2</v>
-      </c>
-      <c r="M3" s="6">
-        <v>6.177672E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="L3" s="4">
+        <f>AVERAGE(-0.03,0.04,-0.01,0.11)</f>
+        <v>2.75E-2</v>
+      </c>
+      <c r="M3" s="4">
+        <f>STDEV(-0.03,0.04,-0.01,0.11)</f>
+        <v>6.2383224240709668E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -712,51 +616,64 @@
         <v>270.22030000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2">
-        <v>0.48680555555555555</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="I4">
-        <v>253</v>
-      </c>
-      <c r="L4" s="7">
-        <v>-8.1818180000000004E-2</v>
-      </c>
-      <c r="M4" s="6">
-        <v>6.177672E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
+        <v>192</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
         <v>44849</v>
       </c>
-      <c r="F5">
-        <v>270.22030000000001</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="I5">
-        <v>192</v>
-      </c>
-      <c r="L5" s="7">
-        <v>-8.1818180000000004E-2</v>
-      </c>
-      <c r="M5" s="6">
-        <v>6.177672E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="7">
+        <v>0.197188</v>
+      </c>
+      <c r="E5" s="7">
+        <v>7.8486669999999998</v>
+      </c>
+      <c r="F5" s="5">
+        <v>386.77969999999999</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="I5" s="5">
+        <v>148</v>
+      </c>
+      <c r="L5" s="5">
+        <f>AVERAGE(-0.09,-0.07,-0.04,-0.04,-0.01,-0.01)</f>
+        <v>-4.3333333333333335E-2</v>
+      </c>
+      <c r="M5" s="5">
+        <f>STDEV(-0.09,-0.07,-0.04,-0.04,-0.01,-0.01)</f>
+        <v>3.2041639575194444E-2</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="O5">
+        <v>62.511800000000001</v>
+      </c>
+      <c r="P5" s="5">
+        <v>6.899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -766,69 +683,41 @@
       <c r="C6" s="1">
         <v>44849</v>
       </c>
-      <c r="D6"/>
-      <c r="E6"/>
       <c r="F6">
         <v>386.77969999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2">
-        <v>0.52222222222222225</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="I6">
-        <v>148</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>44849</v>
       </c>
-      <c r="F7">
-        <v>386.77969999999999</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2">
-        <v>0.52430555555555558</v>
+        <v>0.53194444444444444</v>
       </c>
       <c r="I7">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -840,37 +729,62 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2">
-        <v>0.53194444444444444</v>
+        <v>0.53263888888888888</v>
       </c>
       <c r="I8">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>44849</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="D9" s="3">
+        <v>0.33206950000000002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.5819999999999999</v>
+      </c>
+      <c r="F9">
+        <v>553.2373</v>
+      </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2">
-        <v>0.53263888888888888</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="I9">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE(0.06,0.08,-0.03,-0.01,-0.01,-0.01,0)</f>
+        <v>1.1428571428571432E-2</v>
+      </c>
+      <c r="M9">
+        <f>STDEV(0.06,0.08,-0.03,-0.01,-0.01,-0.01,0)</f>
+        <v>4.1403933560541249E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="O9">
+        <v>62.445</v>
+      </c>
+      <c r="P9">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11</v>
       </c>
@@ -884,39 +798,37 @@
         <v>553.2373</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2">
-        <v>0.55555555555555558</v>
+        <v>0.55763888888888891</v>
       </c>
       <c r="I10">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>44849</v>
       </c>
-      <c r="F11">
-        <v>553.2373</v>
-      </c>
+      <c r="F11" s="2"/>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H11" s="2">
-        <v>0.55763888888888891</v>
+        <v>0.56041666666666667</v>
       </c>
       <c r="I11">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -928,37 +840,54 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2">
-        <v>0.56041666666666667</v>
+        <v>0.56180555555555556</v>
       </c>
       <c r="I12">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>44849</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>44850</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.27829159999999997</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8.2486669999999993</v>
+      </c>
+      <c r="F13">
+        <v>993.44069999999999</v>
+      </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H13" s="2">
-        <v>0.56180555555555556</v>
+        <v>0.37708333333333338</v>
       </c>
       <c r="I13">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="O13">
+        <v>62.280700000000003</v>
+      </c>
+      <c r="P13">
+        <v>6.7960000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -972,39 +901,37 @@
         <v>993.44069999999999</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H14" s="2">
-        <v>0.37708333333333338</v>
+        <v>0.37986111111111115</v>
       </c>
       <c r="I14">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1">
         <v>44850</v>
       </c>
-      <c r="F15">
-        <v>993.44069999999999</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2">
-        <v>0.37986111111111115</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="I15">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1016,37 +943,62 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2">
-        <v>0.39097222222222222</v>
+        <v>0.39305555555555555</v>
       </c>
       <c r="I16">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
         <v>44850</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="D17" s="3">
+        <v>0.3079828</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7.5893329999999999</v>
+      </c>
+      <c r="F17">
+        <v>1715.203</v>
+      </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H17" s="2">
-        <v>0.39305555555555555</v>
+        <v>0.51597222222222217</v>
       </c>
       <c r="I17">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE(0.01,0.04,0.02)</f>
+        <v>2.3333333333333334E-2</v>
+      </c>
+      <c r="M17">
+        <f>STDEV(0.01,0.04,0.02)</f>
+        <v>1.5275252316519466E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="O17">
+        <v>62.4405</v>
+      </c>
+      <c r="P17">
+        <v>6.8209999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1060,39 +1012,37 @@
         <v>1715.203</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H18" s="2">
-        <v>0.51597222222222217</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="I18">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1">
         <v>44850</v>
       </c>
-      <c r="F19">
-        <v>1715.203</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H19" s="2">
-        <v>0.52638888888888891</v>
+        <v>0.54027777777777775</v>
       </c>
       <c r="I19">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1104,37 +1054,62 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2">
-        <v>0.54027777777777775</v>
+        <v>0.54236111111111118</v>
       </c>
       <c r="I20">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
         <v>44850</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="D21" s="3">
+        <v>0.4166301</v>
+      </c>
+      <c r="E21">
+        <v>8.3819999999999997</v>
+      </c>
+      <c r="F21">
+        <v>2569.4920000000002</v>
+      </c>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H21" s="2">
-        <v>0.54236111111111118</v>
+        <v>0.64027777777777783</v>
       </c>
       <c r="I21">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="L21">
+        <f>AVERAGE(0.04,0.04,0.05,0.08)</f>
+        <v>5.2500000000000005E-2</v>
+      </c>
+      <c r="M21">
+        <f>STDEV(0.04,0.04,0.05,0.08)</f>
+        <v>1.8929694486000893E-2</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="O21">
+        <v>62.2806</v>
+      </c>
+      <c r="P21">
+        <v>6.8129999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1148,39 +1123,37 @@
         <v>2569.4920000000002</v>
       </c>
       <c r="G22" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H22" s="2">
-        <v>0.64027777777777783</v>
+        <v>0.64166666666666672</v>
       </c>
       <c r="I22">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1">
         <v>44850</v>
       </c>
-      <c r="F23">
-        <v>2569.4920000000002</v>
-      </c>
+      <c r="F23" s="2"/>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2">
-        <v>0.64166666666666672</v>
+        <v>0.6430555555555556</v>
       </c>
       <c r="I23">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1192,37 +1165,62 @@
       </c>
       <c r="F24" s="2"/>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H24" s="2">
-        <v>0.6430555555555556</v>
+        <v>0.64374999999999993</v>
       </c>
       <c r="I24">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
         <v>44850</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="D25">
+        <v>8.9779999999999998</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.58949039999999997</v>
+      </c>
+      <c r="F25">
+        <v>1981.4580000000001</v>
+      </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H25" s="2">
-        <v>0.64374999999999993</v>
+        <v>0.66805555555555562</v>
       </c>
       <c r="I25">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="L25">
+        <f>AVERAGE(0.11,0.05,0.01,0.01,-0.02,-0.01)</f>
+        <v>2.5000000000000005E-2</v>
+      </c>
+      <c r="M25">
+        <f>STDEV(0.11,0.05,0.01,0.01,-0.02,-0.01)</f>
+        <v>4.8062459362791653E-2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O25">
+        <v>62.2605</v>
+      </c>
+      <c r="P25">
+        <v>6.8070000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1236,39 +1234,37 @@
         <v>1981.4580000000001</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H26" s="2">
         <v>0.66805555555555562</v>
       </c>
       <c r="I26">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1">
         <v>44850</v>
       </c>
-      <c r="F27">
-        <v>1981.4580000000001</v>
-      </c>
+      <c r="F27" s="2"/>
       <c r="G27" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H27" s="2">
-        <v>0.66805555555555562</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="I27">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1280,37 +1276,62 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H28" s="2">
-        <v>0.67013888888888884</v>
+        <v>0.67083333333333339</v>
       </c>
       <c r="I28">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1">
         <v>44850</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="D29">
+        <v>8.4809999999999999</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.60381300000000004</v>
+      </c>
+      <c r="F29">
+        <v>2562.8809999999999</v>
+      </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H29" s="2">
-        <v>0.67083333333333339</v>
+        <v>0.68541666666666667</v>
       </c>
       <c r="I29">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="L29">
+        <f>AVERAGE(0.32,0.28,0.26,0.29,0.23)</f>
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="M29">
+        <f>STDEV(0.32,0.28,0.26,0.29,0.23)</f>
+        <v>3.3615472627943108E-2</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="O29">
+        <v>62.266399999999997</v>
+      </c>
+      <c r="P29">
+        <v>6.8019999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1324,39 +1345,37 @@
         <v>2562.8809999999999</v>
       </c>
       <c r="G30" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2">
-        <v>0.68541666666666667</v>
+        <v>0.6875</v>
       </c>
       <c r="I30">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>9</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1">
         <v>44850</v>
       </c>
-      <c r="F31">
-        <v>2562.8809999999999</v>
-      </c>
+      <c r="F31" s="2"/>
       <c r="G31" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H31" s="2">
-        <v>0.6875</v>
+        <v>0.68888888888888899</v>
       </c>
       <c r="I31">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1368,40 +1387,19 @@
       </c>
       <c r="F32" s="2"/>
       <c r="G32" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H32" s="2">
         <v>0.68888888888888899</v>
       </c>
       <c r="I32">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>9</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1">
-        <v>44850</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0.68888888888888899</v>
-      </c>
-      <c r="I33">
         <v>211</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG37">
-    <sortCondition ref="C2:C37"/>
-    <sortCondition ref="H2:H37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q36">
+    <sortCondition ref="C2:C36"/>
+    <sortCondition ref="H2:H36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>